<commit_message>
Add translations for steel industry plot
</commit_message>
<xml_diff>
--- a/data/label translations.xlsx
+++ b/data/label translations.xlsx
@@ -10,24 +10,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment authorId="0" ref="B100">
-      <text>
-        <t xml:space="preserve">@qi@energyandcleanair.org translations needed
-	-Lauri Myllyvirta</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="219">
   <si>
     <t>EN</t>
   </si>
@@ -599,7 +583,91 @@
     <t>Labels show year-on-year changes for the current year</t>
   </si>
   <si>
-    <t>红色框内显示当年同比变化</t>
+    <t>方框内显示当年同比变化</t>
+  </si>
+  <si>
+    <t>Steel industry weekly operating indicators</t>
+  </si>
+  <si>
+    <t>钢铁行业周运行数据</t>
+  </si>
+  <si>
+    <t>Average Daily Output: Crude Steel</t>
+  </si>
+  <si>
+    <t>平均日产量：粗钢</t>
+  </si>
+  <si>
+    <t>Blast furnace capacity utilization</t>
+  </si>
+  <si>
+    <t>高炉产能利用率</t>
+  </si>
+  <si>
+    <t>Blast furnace starting rate</t>
+  </si>
+  <si>
+    <t>高炉开工率</t>
+  </si>
+  <si>
+    <t>Capacity utilization: Electric Stove</t>
+  </si>
+  <si>
+    <t>产能利用率：电炉</t>
+  </si>
+  <si>
+    <t>Deformed Steel Bar: Operating Rate</t>
+  </si>
+  <si>
+    <t>螺纹钢：开工率</t>
+  </si>
+  <si>
+    <t>Estimated Average Daily Output: Crude Steel</t>
+  </si>
+  <si>
+    <t>平均估算日产量：粗钢</t>
+  </si>
+  <si>
+    <t>Estimated Daily Average Output: Pig Iron</t>
+  </si>
+  <si>
+    <t>平均估算日产量：生铁</t>
+  </si>
+  <si>
+    <t>Estimated Daily Average Output: Steel Products</t>
+  </si>
+  <si>
+    <t>平均估算日产量：钢铁产品</t>
+  </si>
+  <si>
+    <t>Operating Rate of Blast Furnaces: Tangshan</t>
+  </si>
+  <si>
+    <t>高炉开工率：唐山</t>
+  </si>
+  <si>
+    <t>Operating Rate: Electric Furnace</t>
+  </si>
+  <si>
+    <t>开工率：电炉</t>
+  </si>
+  <si>
+    <t>Tangshan: Operating Rate of Blast Furnaces</t>
+  </si>
+  <si>
+    <t>唐山：高炉开工率</t>
+  </si>
+  <si>
+    <t>Wire Rod: Operating Rate of Main Steel Plant</t>
+  </si>
+  <si>
+    <t>线材：主要钢厂开工率</t>
+  </si>
+  <si>
+    <t>Source: Wind Information</t>
+  </si>
+  <si>
+    <t>数据来源：万得资讯</t>
   </si>
 </sst>
 </file>
@@ -1668,8 +1736,119 @@
         <v>190</v>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completed Chinese graph output for 2023Q2 CO2 analysis
</commit_message>
<xml_diff>
--- a/data/label translations.xlsx
+++ b/data/label translations.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="270">
   <si>
     <t>EN</t>
   </si>
@@ -668,13 +668,166 @@
   </si>
   <si>
     <t>数据来源：万得资讯</t>
+  </si>
+  <si>
+    <t>China's CO2 emissions from energy and cement</t>
+  </si>
+  <si>
+    <t>中国化石燃料和水泥的二氧化碳排放量</t>
+  </si>
+  <si>
+    <t>Mt CO2 / quarter</t>
+  </si>
+  <si>
+    <t>亿吨二氧化碳/季度</t>
+  </si>
+  <si>
+    <t>Trends in China CO2 by fuel and sector</t>
+  </si>
+  <si>
+    <t>不同行业化石燃料和水泥的二氧化碳排放量变化趋势</t>
+  </si>
+  <si>
+    <t>pre-COVID trendline</t>
+  </si>
+  <si>
+    <t>疫情前变化趋势</t>
+  </si>
+  <si>
+    <t>First COVID-19 lockdown</t>
+  </si>
+  <si>
+    <t>新冠疫情爆发</t>
+  </si>
+  <si>
+    <t>Mt/year, 12 month moving sum</t>
+  </si>
+  <si>
+    <t>亿吨/年，12个月移动平均值</t>
+  </si>
+  <si>
+    <t>炼焦煤</t>
+  </si>
+  <si>
+    <t>石油产品</t>
+  </si>
+  <si>
+    <t>Steam coal</t>
+  </si>
+  <si>
+    <t>Automobiles</t>
+  </si>
+  <si>
+    <t>New Energy Vehicles</t>
+  </si>
+  <si>
+    <t>Vehicles Production</t>
+  </si>
+  <si>
+    <t>乘用车产量</t>
+  </si>
+  <si>
+    <t>Million units, 12-month moving sum</t>
+  </si>
+  <si>
+    <t>百万辆，12个月移动平均值</t>
+  </si>
+  <si>
+    <t>cumulative sales over 10 years</t>
+  </si>
+  <si>
+    <t>过去十年总销量</t>
+  </si>
+  <si>
+    <t>new sales, 3-month mean</t>
+  </si>
+  <si>
+    <t>新车总销量，三个月平均值</t>
+  </si>
+  <si>
+    <t>新能源车占比</t>
+  </si>
+  <si>
+    <t>Power Sector Coal Consumption in China</t>
+  </si>
+  <si>
+    <t>电力行业煤炭消耗量</t>
+  </si>
+  <si>
+    <t>Mt/year, 12-month moving sum</t>
+  </si>
+  <si>
+    <t>predicted based on output</t>
+  </si>
+  <si>
+    <t>根据产量测算</t>
+  </si>
+  <si>
+    <t>reported</t>
+  </si>
+  <si>
+    <t>公布的数据</t>
+  </si>
+  <si>
+    <t>without drought&amp;heatwave</t>
+  </si>
+  <si>
+    <t>剔除干旱和水电产量下降因素</t>
+  </si>
+  <si>
+    <t>All Sectors</t>
+  </si>
+  <si>
+    <t>所有行业</t>
+  </si>
+  <si>
+    <t>Non-power use</t>
+  </si>
+  <si>
+    <t>非电力用途</t>
+  </si>
+  <si>
+    <t>Power Industry</t>
+  </si>
+  <si>
+    <t>电力行业</t>
+  </si>
+  <si>
+    <t>Metallurgy Industry</t>
+  </si>
+  <si>
+    <t>冶金行业</t>
+  </si>
+  <si>
+    <t>Quarterly</t>
+  </si>
+  <si>
+    <t>每季度</t>
+  </si>
+  <si>
+    <t>Mt/year</t>
+  </si>
+  <si>
+    <t>亿吨/年</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Coal consumption in China</t>
+  </si>
+  <si>
+    <t>煤炭消耗量</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -686,13 +839,24 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="&quot;Google Sans&quot;"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -701,11 +865,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1848,6 +2015,294 @@
         <v>218</v>
       </c>
     </row>
+    <row r="116">
+      <c r="A116" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>